<commit_message>
on croyait que c'était fini mais en fait non
</commit_message>
<xml_diff>
--- a/code/notebooks/sortie_jalon3.xlsx
+++ b/code/notebooks/sortie_jalon3.xlsx
@@ -2104,7 +2104,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D631"/>
+  <dimension ref="A1:D671"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10951,6 +10951,566 @@
         <v>0</v>
       </c>
       <c r="D631" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" s="2" t="n">
+        <v>44787.5625</v>
+      </c>
+      <c r="B632" t="n">
+        <v>0</v>
+      </c>
+      <c r="C632" t="n">
+        <v>0</v>
+      </c>
+      <c r="D632" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" s="2" t="n">
+        <v>44787.57291666666</v>
+      </c>
+      <c r="B633" t="n">
+        <v>0</v>
+      </c>
+      <c r="C633" t="n">
+        <v>0</v>
+      </c>
+      <c r="D633" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" s="2" t="n">
+        <v>44787.58333333334</v>
+      </c>
+      <c r="B634" t="n">
+        <v>0</v>
+      </c>
+      <c r="C634" t="n">
+        <v>0</v>
+      </c>
+      <c r="D634" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" s="2" t="n">
+        <v>44787.59375</v>
+      </c>
+      <c r="B635" t="n">
+        <v>0</v>
+      </c>
+      <c r="C635" t="n">
+        <v>0</v>
+      </c>
+      <c r="D635" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" s="2" t="n">
+        <v>44787.60416666666</v>
+      </c>
+      <c r="B636" t="n">
+        <v>0</v>
+      </c>
+      <c r="C636" t="n">
+        <v>0</v>
+      </c>
+      <c r="D636" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" s="2" t="n">
+        <v>44787.61458333334</v>
+      </c>
+      <c r="B637" t="n">
+        <v>0</v>
+      </c>
+      <c r="C637" t="n">
+        <v>0</v>
+      </c>
+      <c r="D637" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" s="2" t="n">
+        <v>44787.625</v>
+      </c>
+      <c r="B638" t="n">
+        <v>0</v>
+      </c>
+      <c r="C638" t="n">
+        <v>0</v>
+      </c>
+      <c r="D638" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" s="2" t="n">
+        <v>44787.63541666666</v>
+      </c>
+      <c r="B639" t="n">
+        <v>0</v>
+      </c>
+      <c r="C639" t="n">
+        <v>0</v>
+      </c>
+      <c r="D639" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" s="2" t="n">
+        <v>44787.64583333334</v>
+      </c>
+      <c r="B640" t="n">
+        <v>0</v>
+      </c>
+      <c r="C640" t="n">
+        <v>0</v>
+      </c>
+      <c r="D640" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" s="2" t="n">
+        <v>44787.65625</v>
+      </c>
+      <c r="B641" t="n">
+        <v>0</v>
+      </c>
+      <c r="C641" t="n">
+        <v>0</v>
+      </c>
+      <c r="D641" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" s="2" t="n">
+        <v>44787.66666666666</v>
+      </c>
+      <c r="B642" t="n">
+        <v>0</v>
+      </c>
+      <c r="C642" t="n">
+        <v>0</v>
+      </c>
+      <c r="D642" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" s="2" t="n">
+        <v>44787.67708333334</v>
+      </c>
+      <c r="B643" t="n">
+        <v>0</v>
+      </c>
+      <c r="C643" t="n">
+        <v>0</v>
+      </c>
+      <c r="D643" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" s="2" t="n">
+        <v>44787.6875</v>
+      </c>
+      <c r="B644" t="n">
+        <v>0</v>
+      </c>
+      <c r="C644" t="n">
+        <v>0</v>
+      </c>
+      <c r="D644" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" s="2" t="n">
+        <v>44787.69791666666</v>
+      </c>
+      <c r="B645" t="n">
+        <v>0</v>
+      </c>
+      <c r="C645" t="n">
+        <v>0</v>
+      </c>
+      <c r="D645" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" s="2" t="n">
+        <v>44787.70833333334</v>
+      </c>
+      <c r="B646" t="n">
+        <v>0</v>
+      </c>
+      <c r="C646" t="n">
+        <v>0</v>
+      </c>
+      <c r="D646" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" s="2" t="n">
+        <v>44787.71875</v>
+      </c>
+      <c r="B647" t="n">
+        <v>0</v>
+      </c>
+      <c r="C647" t="n">
+        <v>0</v>
+      </c>
+      <c r="D647" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" s="2" t="n">
+        <v>44787.72916666666</v>
+      </c>
+      <c r="B648" t="n">
+        <v>0</v>
+      </c>
+      <c r="C648" t="n">
+        <v>0</v>
+      </c>
+      <c r="D648" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" s="2" t="n">
+        <v>44787.73958333334</v>
+      </c>
+      <c r="B649" t="n">
+        <v>0</v>
+      </c>
+      <c r="C649" t="n">
+        <v>0</v>
+      </c>
+      <c r="D649" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" s="2" t="n">
+        <v>44787.75</v>
+      </c>
+      <c r="B650" t="n">
+        <v>0</v>
+      </c>
+      <c r="C650" t="n">
+        <v>0</v>
+      </c>
+      <c r="D650" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" s="2" t="n">
+        <v>44787.76041666666</v>
+      </c>
+      <c r="B651" t="n">
+        <v>0</v>
+      </c>
+      <c r="C651" t="n">
+        <v>0</v>
+      </c>
+      <c r="D651" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" s="2" t="n">
+        <v>44787.77083333334</v>
+      </c>
+      <c r="B652" t="n">
+        <v>0</v>
+      </c>
+      <c r="C652" t="n">
+        <v>0</v>
+      </c>
+      <c r="D652" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" s="2" t="n">
+        <v>44787.78125</v>
+      </c>
+      <c r="B653" t="n">
+        <v>0</v>
+      </c>
+      <c r="C653" t="n">
+        <v>0</v>
+      </c>
+      <c r="D653" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" s="2" t="n">
+        <v>44787.79166666666</v>
+      </c>
+      <c r="B654" t="n">
+        <v>0</v>
+      </c>
+      <c r="C654" t="n">
+        <v>0</v>
+      </c>
+      <c r="D654" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" s="2" t="n">
+        <v>44787.80208333334</v>
+      </c>
+      <c r="B655" t="n">
+        <v>0</v>
+      </c>
+      <c r="C655" t="n">
+        <v>0</v>
+      </c>
+      <c r="D655" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" s="2" t="n">
+        <v>44787.8125</v>
+      </c>
+      <c r="B656" t="n">
+        <v>0</v>
+      </c>
+      <c r="C656" t="n">
+        <v>0</v>
+      </c>
+      <c r="D656" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" s="2" t="n">
+        <v>44787.82291666666</v>
+      </c>
+      <c r="B657" t="n">
+        <v>0</v>
+      </c>
+      <c r="C657" t="n">
+        <v>0</v>
+      </c>
+      <c r="D657" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" s="2" t="n">
+        <v>44787.83333333334</v>
+      </c>
+      <c r="B658" t="n">
+        <v>0</v>
+      </c>
+      <c r="C658" t="n">
+        <v>0</v>
+      </c>
+      <c r="D658" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" s="2" t="n">
+        <v>44787.84375</v>
+      </c>
+      <c r="B659" t="n">
+        <v>0</v>
+      </c>
+      <c r="C659" t="n">
+        <v>0</v>
+      </c>
+      <c r="D659" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" s="2" t="n">
+        <v>44787.85416666666</v>
+      </c>
+      <c r="B660" t="n">
+        <v>0</v>
+      </c>
+      <c r="C660" t="n">
+        <v>0</v>
+      </c>
+      <c r="D660" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" s="2" t="n">
+        <v>44787.86458333334</v>
+      </c>
+      <c r="B661" t="n">
+        <v>0</v>
+      </c>
+      <c r="C661" t="n">
+        <v>0</v>
+      </c>
+      <c r="D661" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" s="2" t="n">
+        <v>44787.875</v>
+      </c>
+      <c r="B662" t="n">
+        <v>0</v>
+      </c>
+      <c r="C662" t="n">
+        <v>0</v>
+      </c>
+      <c r="D662" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" s="2" t="n">
+        <v>44787.88541666666</v>
+      </c>
+      <c r="B663" t="n">
+        <v>0</v>
+      </c>
+      <c r="C663" t="n">
+        <v>0</v>
+      </c>
+      <c r="D663" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" s="2" t="n">
+        <v>44787.89583333334</v>
+      </c>
+      <c r="B664" t="n">
+        <v>0</v>
+      </c>
+      <c r="C664" t="n">
+        <v>0</v>
+      </c>
+      <c r="D664" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" s="2" t="n">
+        <v>44787.90625</v>
+      </c>
+      <c r="B665" t="n">
+        <v>0</v>
+      </c>
+      <c r="C665" t="n">
+        <v>0</v>
+      </c>
+      <c r="D665" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" s="2" t="n">
+        <v>44787.91666666666</v>
+      </c>
+      <c r="B666" t="n">
+        <v>0</v>
+      </c>
+      <c r="C666" t="n">
+        <v>0</v>
+      </c>
+      <c r="D666" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" s="2" t="n">
+        <v>44787.92708333334</v>
+      </c>
+      <c r="B667" t="n">
+        <v>0</v>
+      </c>
+      <c r="C667" t="n">
+        <v>0</v>
+      </c>
+      <c r="D667" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" s="2" t="n">
+        <v>44787.9375</v>
+      </c>
+      <c r="B668" t="n">
+        <v>0</v>
+      </c>
+      <c r="C668" t="n">
+        <v>0</v>
+      </c>
+      <c r="D668" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" s="2" t="n">
+        <v>44787.94791666666</v>
+      </c>
+      <c r="B669" t="n">
+        <v>0</v>
+      </c>
+      <c r="C669" t="n">
+        <v>0</v>
+      </c>
+      <c r="D669" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" s="2" t="n">
+        <v>44787.95833333334</v>
+      </c>
+      <c r="B670" t="n">
+        <v>0</v>
+      </c>
+      <c r="C670" t="n">
+        <v>0</v>
+      </c>
+      <c r="D670" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" s="2" t="n">
+        <v>44787.96875</v>
+      </c>
+      <c r="B671" t="n">
+        <v>0</v>
+      </c>
+      <c r="C671" t="n">
+        <v>0</v>
+      </c>
+      <c r="D671" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>